<commit_message>
Debug. Num scenarios reduced.
</commit_message>
<xml_diff>
--- a/data/CS5/Market Data/CS5_market_data_2045.xlsx
+++ b/data/CS5/Market Data/CS5_market_data_2045.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE5FFCE-960B-4598-BA7E-E244EA4E7A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD863C4-2F90-4771-925F-D06F700C54E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,19 +1335,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
         <f>1/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>